<commit_message>
Add action table to report
</commit_message>
<xml_diff>
--- a/ActionTable.xlsx
+++ b/ActionTable.xlsx
@@ -548,7 +548,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH28" sqref="AH28"/>
+      <selection pane="topRight" activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,14 +697,14 @@
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
         <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
       </c>
       <c r="P4">
         <v>3</v>
@@ -742,11 +742,11 @@
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
       <c r="C7">
         <v>7</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
       </c>
       <c r="P7">
         <v>7</v>

</xml_diff>

<commit_message>
Add actionTable to the project
</commit_message>
<xml_diff>
--- a/ActionTable.xlsx
+++ b/ActionTable.xlsx
@@ -547,8 +547,8 @@
   <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG1" sqref="AG1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,22 +1073,22 @@
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <v>40</v>
+      </c>
+      <c r="J24">
+        <v>40</v>
+      </c>
+      <c r="L24">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C25">
-        <v>40</v>
-      </c>
-      <c r="E25">
-        <v>40</v>
-      </c>
-      <c r="J25">
-        <v>40</v>
-      </c>
-      <c r="L25">
-        <v>40</v>
       </c>
       <c r="W25">
         <v>41</v>

</xml_diff>

<commit_message>
Fix actionTable in cond
</commit_message>
<xml_diff>
--- a/ActionTable.xlsx
+++ b/ActionTable.xlsx
@@ -547,8 +547,8 @@
   <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" sqref="A12:XFD12"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +731,7 @@
       <c r="A6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6">
+      <c r="H6">
         <v>5</v>
       </c>
       <c r="AG6">

</xml_diff>